<commit_message>
Reverting pull request 330 to commit 261d95fc12 [formerly 0a7c0c1fcb]
261d95fc128052400b2f5ba2eb0b61776abc3cee [formerly 0a7c0c1fcb777bc593812010a0a903c190a68188]

Former-commit-id: b17bed75a777bb56e4931307475cc8fa8a1577ed
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Partner Management Requirements.xlsx
+++ b/docs/requirements/MOSIP_Partner Management Requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Sr No.</t>
   </si>
@@ -85,84 +85,16 @@
     <t>Partner ID Validation</t>
   </si>
   <si>
-    <t>1. Validate length of a Partner ID as configured and respond as mentioned below
-a. If found valid, respond with "Valid"
-b. if found invalid, respond with "Invalid"</t>
-  </si>
-  <si>
-    <t>1. Validate length of a License Key as configured and respond as mentioned below
-a. If found valid, respond with "Valid"
-b. if found invalid, respond with "Invalid"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kernel </t>
   </si>
   <si>
-    <t>Policy ID Generation</t>
-  </si>
-  <si>
-    <t>1. Generate Policy ID for following policies
-a. OTP Trigger 
-b. OTP Authentication
-c. Demo Authentication 
-d. Biometric Authentication - FMR Data Match 
-e. Biometric Authentication - IIR Data Match  
-f. Biometric Authentication - FID Data Match 
-g. Static Pin Authentication
-h. eKYC - all combinations of eKYC demo fields 
-i. Masked UIN
-j. UIN
-2. Generate Policy id as per below logic
-a. Random ID generation
-b. Length should be 10 Digits (Configurable)</t>
-  </si>
-  <si>
-    <t>Policy ID Validation</t>
-  </si>
-  <si>
-    <t>1. Validate length of a Policy ID as configured and respond as mentioned below
-a. If found valid, respond with "Valid"
-b. if found invalid, respond with "Invalid"</t>
-  </si>
-  <si>
-    <t>Policy ID</t>
-  </si>
-  <si>
-    <t>1. Receive request to retreive policies based on Partner ID and Policy ID
-2. Respond appropirately if Partner ID or Policy ID does not exist</t>
-  </si>
-  <si>
     <t>Partner Registration</t>
   </si>
   <si>
     <t>MISP - Partner Mapping</t>
   </si>
   <si>
-    <t>1. Receive a request to map MISP to a Partner with MISP ID and Partner ID as Input
-2. There can ve a many-to-mapping between MISPs and Partners</t>
-  </si>
-  <si>
-    <t>Partner Certiicate Validation</t>
-  </si>
-  <si>
-    <t>Partner Certificate Signing and RE-issueing</t>
-  </si>
-  <si>
-    <t>1. Receive certificate from Partner
-2. Verify CA Authority of the certificate</t>
-  </si>
-  <si>
     <t>Distribution of Public Key to Partners</t>
-  </si>
-  <si>
-    <t>1. Distribute Public Key to Partners correspinding to the Private Key used to signed the Certificate
-2. Public key needs to be distributed priodically whenever the Private Key is rotated</t>
-  </si>
-  <si>
-    <t>1. Receive certificate from Partner during Partner Registration
-2. Sign the Partner Certificate with MOSIP Private Key and issue a certificate chain
-3. Re-issue certficate back to the Partner
-4. Private key to change priodically as per the Key Rotation Policy set by admin</t>
   </si>
   <si>
     <t>Device Registration</t>
@@ -182,6 +114,24 @@
 b. License Key should be alphanumeric
 c. Length should be 8 digits (Configurable)
 d. Should be mapped to an expiry</t>
+  </si>
+  <si>
+    <t>Yet to analyzed</t>
+  </si>
+  <si>
+    <t>Component already exist as TSP ID generator</t>
+  </si>
+  <si>
+    <t>Partner Management (MISP and E-KYC/Auth Partners)</t>
+  </si>
+  <si>
+    <t>1. Validate status of Lisence Key and respond as mentioned below
+a. If found expired, respond with "Your License Key is EXPIRED. Please regenrate a new License Key"
+b. If found temporarily sespended, respond with "Your License Key is temporarily SUSPENDED. Please contact MOSIP Administration"
+c. If found permanently blocked, respond with "Your License Key is BLOCKED. Please contact MOSIP Administration"</t>
+  </si>
+  <si>
+    <t>Map Policies to Partners</t>
   </si>
   <si>
     <t>1. Receive request to register a Partner with follwing parameters
@@ -190,25 +140,58 @@
 c. Partner Phone
 d. Partner Email ID
 2. Issue and Map Partner ID
-3. Map Policy ID to the Partner
+3. Map Policies to the Partner
 a. Multiple Policies can be mapped to a Partner
 b. A Partner can have a policy for both Auth and E-KYC
 4. Store the Partner in MOSIP</t>
   </si>
   <si>
-    <t>Yet to analyzed</t>
-  </si>
-  <si>
-    <t>Component already exist as TSP ID generator</t>
-  </si>
-  <si>
-    <t>Partner Management (MISP and E-KYC/Auth Partners)</t>
-  </si>
-  <si>
-    <t>1. Validate status of Lisence Key and respond as mentioned below
-a. If found expired, respond with "Your License Key is EXPIRED. Please regenrate a new License Key"
-b. If found temporarily sespended, respond with "Your License Key is temporarily SUSPENDED. Please contact MOSIP Administration"
-c. If found permanently blocked, respond with "Your License Key is BLOCKED. Please contact MOSIP Administration"</t>
+    <t>Retrieve Policies based on Partner ID</t>
+  </si>
+  <si>
+    <t>1. Receive a request to map MISP to a Partner with MISP ID and Partner ID as Input
+2. There can be a many-to-mapping between MISPs and Partners</t>
+  </si>
+  <si>
+    <t>Partner Certificate Validation</t>
+  </si>
+  <si>
+    <t>1. Distribute Public Key to Partners for encrypting the Auth Request befoe sending it to the MOSIP
+2. Public key needs to be distributed priodically whenever the correspinding Private Key is rotated</t>
+  </si>
+  <si>
+    <t>1. Validate length of a License Key as configured and respond as mentioned below
+a. If found valid, respond with "VALID"
+b. if found invalid, respond with "INVALID"</t>
+  </si>
+  <si>
+    <t>1. Validate length of a Partner ID as configured and respond as mentioned below
+a. If found valid, respond with "VALID"
+b. if found invalid, respond with "INVALID"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Map following Policies to Partners
+a. Auth Policies ( can be Mandatory/Non-Mandatory)
+     1. OTP Trigger 
+     2. OTP Authentication
+     3. Demo Authentication 
+     4. Biometric Authentication - FMR Data Match 
+     5. Biometric Authentication - IIR Data Match  
+     6. Biometric Authentication - FID Data Match 
+b. E-Kyc Policies (can be Required/Not Required)
+    1. eKYC - all combinations of eKYC demo fields </t>
+  </si>
+  <si>
+    <t>1. Receive request to retreive policies based on Partner ID
+2. Respond appropirately if Partner ID does not exist</t>
+  </si>
+  <si>
+    <t>1. Upload Digital Certificate on Admin Portal for a Partner
+2. Verify CA Authority of the certificate
+3. Sign the certificate with MOSIP Certificate
+4. Respond to the source with the re-issued certificate
+5. Certificate will be uploaded by the MOSIP admin. The Registered Partner will send the certificate to the MOSIP Admin through ofline process. Re-issued certificate will be sent to the Partner by MOSIP admin through notification/offline process
+6. Private key to change priodically as per the Key Rotation Policy set by admin</t>
   </si>
 </sst>
 </file>
@@ -450,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -461,9 +444,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -495,29 +475,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -641,6 +598,29 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -657,14 +637,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F20" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="B2:F20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F18" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="B2:F18"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sr No." dataDxfId="6"/>
-    <tableColumn id="2" name="Module" dataDxfId="5"/>
-    <tableColumn id="3" name="Feature" dataDxfId="4"/>
-    <tableColumn id="4" name="Acceptance Criteria" dataDxfId="3"/>
-    <tableColumn id="5" name="Comments" dataDxfId="2"/>
+    <tableColumn id="1" name="Sr No." dataDxfId="4"/>
+    <tableColumn id="2" name="Module" dataDxfId="3"/>
+    <tableColumn id="3" name="Feature" dataDxfId="2"/>
+    <tableColumn id="4" name="Acceptance Criteria" dataDxfId="1"/>
+    <tableColumn id="5" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -933,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F20"/>
+  <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -949,28 +929,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -984,11 +964,11 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
@@ -1002,7 +982,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -1017,7 +997,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1032,7 +1012,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1077,179 +1057,149 @@
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="203" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="145" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" ht="145" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="145" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="58" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" ht="87" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="4">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="8">
+        <v>18</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="4">
-        <v>17</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="9">
-        <v>18</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>41</v>
+      <c r="D18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Reverting pull request 330 to commit 261d95fc12 [formerly 0a7c0c1fcb]" Reverting due to compilation failure in kernel-auth This reverts commit 577bb2ff8b1f9c8c8efcd01c78ec268d04d2e128 [formerly b17bed75a777bb56e4931307475cc8fa8a1577ed].
https://mosipid.atlassian.net/browse/Revert "R

Former-commit-id: 805e7dec0c93886319c51be0fc8222fabf286ffe
</commit_message>
<xml_diff>
--- a/docs/requirements/MOSIP_Partner Management Requirements.xlsx
+++ b/docs/requirements/MOSIP_Partner Management Requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Sr No.</t>
   </si>
@@ -85,16 +85,84 @@
     <t>Partner ID Validation</t>
   </si>
   <si>
+    <t>1. Validate length of a Partner ID as configured and respond as mentioned below
+a. If found valid, respond with "Valid"
+b. if found invalid, respond with "Invalid"</t>
+  </si>
+  <si>
+    <t>1. Validate length of a License Key as configured and respond as mentioned below
+a. If found valid, respond with "Valid"
+b. if found invalid, respond with "Invalid"</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kernel </t>
   </si>
   <si>
+    <t>Policy ID Generation</t>
+  </si>
+  <si>
+    <t>1. Generate Policy ID for following policies
+a. OTP Trigger 
+b. OTP Authentication
+c. Demo Authentication 
+d. Biometric Authentication - FMR Data Match 
+e. Biometric Authentication - IIR Data Match  
+f. Biometric Authentication - FID Data Match 
+g. Static Pin Authentication
+h. eKYC - all combinations of eKYC demo fields 
+i. Masked UIN
+j. UIN
+2. Generate Policy id as per below logic
+a. Random ID generation
+b. Length should be 10 Digits (Configurable)</t>
+  </si>
+  <si>
+    <t>Policy ID Validation</t>
+  </si>
+  <si>
+    <t>1. Validate length of a Policy ID as configured and respond as mentioned below
+a. If found valid, respond with "Valid"
+b. if found invalid, respond with "Invalid"</t>
+  </si>
+  <si>
+    <t>Policy ID</t>
+  </si>
+  <si>
+    <t>1. Receive request to retreive policies based on Partner ID and Policy ID
+2. Respond appropirately if Partner ID or Policy ID does not exist</t>
+  </si>
+  <si>
     <t>Partner Registration</t>
   </si>
   <si>
     <t>MISP - Partner Mapping</t>
   </si>
   <si>
+    <t>1. Receive a request to map MISP to a Partner with MISP ID and Partner ID as Input
+2. There can ve a many-to-mapping between MISPs and Partners</t>
+  </si>
+  <si>
+    <t>Partner Certiicate Validation</t>
+  </si>
+  <si>
+    <t>Partner Certificate Signing and RE-issueing</t>
+  </si>
+  <si>
+    <t>1. Receive certificate from Partner
+2. Verify CA Authority of the certificate</t>
+  </si>
+  <si>
     <t>Distribution of Public Key to Partners</t>
+  </si>
+  <si>
+    <t>1. Distribute Public Key to Partners correspinding to the Private Key used to signed the Certificate
+2. Public key needs to be distributed priodically whenever the Private Key is rotated</t>
+  </si>
+  <si>
+    <t>1. Receive certificate from Partner during Partner Registration
+2. Sign the Partner Certificate with MOSIP Private Key and issue a certificate chain
+3. Re-issue certficate back to the Partner
+4. Private key to change priodically as per the Key Rotation Policy set by admin</t>
   </si>
   <si>
     <t>Device Registration</t>
@@ -114,24 +182,6 @@
 b. License Key should be alphanumeric
 c. Length should be 8 digits (Configurable)
 d. Should be mapped to an expiry</t>
-  </si>
-  <si>
-    <t>Yet to analyzed</t>
-  </si>
-  <si>
-    <t>Component already exist as TSP ID generator</t>
-  </si>
-  <si>
-    <t>Partner Management (MISP and E-KYC/Auth Partners)</t>
-  </si>
-  <si>
-    <t>1. Validate status of Lisence Key and respond as mentioned below
-a. If found expired, respond with "Your License Key is EXPIRED. Please regenrate a new License Key"
-b. If found temporarily sespended, respond with "Your License Key is temporarily SUSPENDED. Please contact MOSIP Administration"
-c. If found permanently blocked, respond with "Your License Key is BLOCKED. Please contact MOSIP Administration"</t>
-  </si>
-  <si>
-    <t>Map Policies to Partners</t>
   </si>
   <si>
     <t>1. Receive request to register a Partner with follwing parameters
@@ -140,58 +190,25 @@
 c. Partner Phone
 d. Partner Email ID
 2. Issue and Map Partner ID
-3. Map Policies to the Partner
+3. Map Policy ID to the Partner
 a. Multiple Policies can be mapped to a Partner
 b. A Partner can have a policy for both Auth and E-KYC
 4. Store the Partner in MOSIP</t>
   </si>
   <si>
-    <t>Retrieve Policies based on Partner ID</t>
-  </si>
-  <si>
-    <t>1. Receive a request to map MISP to a Partner with MISP ID and Partner ID as Input
-2. There can be a many-to-mapping between MISPs and Partners</t>
-  </si>
-  <si>
-    <t>Partner Certificate Validation</t>
-  </si>
-  <si>
-    <t>1. Distribute Public Key to Partners for encrypting the Auth Request befoe sending it to the MOSIP
-2. Public key needs to be distributed priodically whenever the correspinding Private Key is rotated</t>
-  </si>
-  <si>
-    <t>1. Validate length of a License Key as configured and respond as mentioned below
-a. If found valid, respond with "VALID"
-b. if found invalid, respond with "INVALID"</t>
-  </si>
-  <si>
-    <t>1. Validate length of a Partner ID as configured and respond as mentioned below
-a. If found valid, respond with "VALID"
-b. if found invalid, respond with "INVALID"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Map following Policies to Partners
-a. Auth Policies ( can be Mandatory/Non-Mandatory)
-     1. OTP Trigger 
-     2. OTP Authentication
-     3. Demo Authentication 
-     4. Biometric Authentication - FMR Data Match 
-     5. Biometric Authentication - IIR Data Match  
-     6. Biometric Authentication - FID Data Match 
-b. E-Kyc Policies (can be Required/Not Required)
-    1. eKYC - all combinations of eKYC demo fields </t>
-  </si>
-  <si>
-    <t>1. Receive request to retreive policies based on Partner ID
-2. Respond appropirately if Partner ID does not exist</t>
-  </si>
-  <si>
-    <t>1. Upload Digital Certificate on Admin Portal for a Partner
-2. Verify CA Authority of the certificate
-3. Sign the certificate with MOSIP Certificate
-4. Respond to the source with the re-issued certificate
-5. Certificate will be uploaded by the MOSIP admin. The Registered Partner will send the certificate to the MOSIP Admin through ofline process. Re-issued certificate will be sent to the Partner by MOSIP admin through notification/offline process
-6. Private key to change priodically as per the Key Rotation Policy set by admin</t>
+    <t>Yet to analyzed</t>
+  </si>
+  <si>
+    <t>Component already exist as TSP ID generator</t>
+  </si>
+  <si>
+    <t>Partner Management (MISP and E-KYC/Auth Partners)</t>
+  </si>
+  <si>
+    <t>1. Validate status of Lisence Key and respond as mentioned below
+a. If found expired, respond with "Your License Key is EXPIRED. Please regenrate a new License Key"
+b. If found temporarily sespended, respond with "Your License Key is temporarily SUSPENDED. Please contact MOSIP Administration"
+c. If found permanently blocked, respond with "Your License Key is BLOCKED. Please contact MOSIP Administration"</t>
   </si>
 </sst>
 </file>
@@ -433,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -444,6 +461,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -475,6 +495,29 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -598,29 +641,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -637,14 +657,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F18" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="B2:F18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F20" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="B2:F20"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sr No." dataDxfId="4"/>
-    <tableColumn id="2" name="Module" dataDxfId="3"/>
-    <tableColumn id="3" name="Feature" dataDxfId="2"/>
-    <tableColumn id="4" name="Acceptance Criteria" dataDxfId="1"/>
-    <tableColumn id="5" name="Comments" dataDxfId="0"/>
+    <tableColumn id="1" name="Sr No." dataDxfId="6"/>
+    <tableColumn id="2" name="Module" dataDxfId="5"/>
+    <tableColumn id="3" name="Feature" dataDxfId="4"/>
+    <tableColumn id="4" name="Acceptance Criteria" dataDxfId="3"/>
+    <tableColumn id="5" name="Comments" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -913,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F18"/>
+  <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -929,28 +949,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -964,11 +984,11 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="72.5" x14ac:dyDescent="0.35">
@@ -982,7 +1002,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -997,7 +1017,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F5" s="7"/>
     </row>
@@ -1012,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F6" s="7"/>
     </row>
@@ -1057,149 +1077,179 @@
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="2:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="203" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="58" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
         <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="2:6" ht="145" x14ac:dyDescent="0.35">
-      <c r="B12" s="4">
-        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" ht="145" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="2:6" ht="145" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="2:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="87" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="2:6" ht="58" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>26</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" s="8">
+      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="9">
         <v>18</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>26</v>
+      <c r="D20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>